<commit_message>
Update for set 7 tests
</commit_message>
<xml_diff>
--- a/Test Summaries/Test Summary 11-07-19 4 kilobytes.xlsx
+++ b/Test Summaries/Test Summary 11-07-19 4 kilobytes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalee\Documents\Work\City University\Performance Testing\Test Summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E853B0D-6CAD-4C2D-9C34-7970E7501E4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952CA776-A2F4-4912-A25D-FC853B7215EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>